<commit_message>
pequenos ajustes para criar um novo evento de formacao de relatorio
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vscode\impressao inteligente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DW\vscode\Impressao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>copias</t>
   </si>
@@ -35,25 +35,85 @@
     <t>pagamento</t>
   </si>
   <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>br</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
     <t>pix</t>
   </si>
   <si>
     <t>dinheiro</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Ricoh</t>
+  </si>
+  <si>
+    <t>Total Mensal</t>
+  </si>
+  <si>
+    <t>Copias</t>
+  </si>
+  <si>
+    <t>Perdas</t>
+  </si>
+  <si>
+    <t>Copias Totais</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pagamento </t>
+  </si>
+  <si>
+    <t>Pix</t>
+  </si>
+  <si>
+    <t>Dinheiro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t>Contador Brother</t>
+  </si>
+  <si>
+    <t>Contador Ricoh</t>
+  </si>
+  <si>
+    <t>Assinaturas dos responsaveis:</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Copias Br</t>
+  </si>
+  <si>
+    <t>Copias Ri</t>
+  </si>
+  <si>
+    <t>Perdas Br</t>
+  </si>
+  <si>
+    <t>Perdas Ri</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -79,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -87,20 +147,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,73 +731,619 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="2"/>
       <c r="M17" s="1"/>
     </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>18</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>24</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>26</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>27</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>28</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>30</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="27"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="19"/>
+      <c r="H38" s="28"/>
+      <c r="I38" s="29"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="H39" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="22"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="19"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="23"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="H41" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="19"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="23"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="31" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="22">
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H37:I38"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -467,12 +1363,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
criandoa a logica que monta os dados diarios
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mensal" sheetId="1" r:id="rId1"/>
@@ -405,51 +405,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,35 +733,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="16" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="16" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="16" t="s">
+      <c r="G1" s="30"/>
+      <c r="H1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
+      <c r="A2" s="31"/>
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1209,72 +1209,72 @@
       <c r="I33" s="13"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="26" t="s">
+      <c r="H37" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="27"/>
+      <c r="I37" s="23"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="19"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="29"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="26"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="25"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="H39" s="24" t="s">
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="H39" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="I39" s="22"/>
+      <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="19"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="23"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="19"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="H41" s="24" t="s">
+      <c r="C41" s="27"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
+      <c r="H41" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="22" t="s">
+      <c r="I41" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="19"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="23"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="19"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -1282,48 +1282,53 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="31" t="s">
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31" t="s">
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="17" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="31" t="s">
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="17" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H37:I38"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="D39:D40"/>
@@ -1331,16 +1336,11 @@
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="E41:E42"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H37:I38"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1365,7 +1365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
relatorio mensal atualizado + botao apagar desabilitado precisando de reparo
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Mensal" sheetId="1" r:id="rId1"/>
     <sheet name="Analise" sheetId="2" r:id="rId2"/>
     <sheet name="Banco de Dados" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>copias</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Dinheiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                                                                                                                                        </t>
   </si>
   <si>
     <t>Contador Brother</t>
@@ -376,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -396,9 +393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -409,18 +403,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -433,24 +439,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,35 +724,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="29" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="29" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="30"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
@@ -781,13 +772,13 @@
         <v>8</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -797,11 +788,11 @@
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>2</v>
       </c>
@@ -811,10 +802,10 @@
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="13"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4" s="27"/>
+      <c r="I4" s="29"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -824,10 +815,10 @@
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5" s="27"/>
+      <c r="I5" s="29"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -837,10 +828,10 @@
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H6" s="27"/>
+      <c r="I6" s="29"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -850,10 +841,10 @@
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="27"/>
+      <c r="I7" s="29"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -863,10 +854,10 @@
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="27"/>
+      <c r="I8" s="29"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -876,10 +867,10 @@
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H9" s="27"/>
+      <c r="I9" s="29"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -889,10 +880,11 @@
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H10" s="27"/>
+      <c r="I10" s="29"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -902,10 +894,10 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="27"/>
+      <c r="I11" s="29"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>10</v>
       </c>
@@ -915,10 +907,10 @@
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="27"/>
+      <c r="I12" s="29"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -928,10 +920,10 @@
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="27"/>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>12</v>
       </c>
@@ -941,10 +933,10 @@
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="27"/>
+      <c r="I14" s="29"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -954,10 +946,10 @@
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="27"/>
+      <c r="I15" s="29"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>14</v>
       </c>
@@ -967,8 +959,8 @@
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="13"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
@@ -980,8 +972,8 @@
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="13"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="29"/>
       <c r="J17" s="2"/>
       <c r="M17" s="1"/>
     </row>
@@ -995,8 +987,8 @@
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="13"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="29"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1009,8 +1001,8 @@
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="13"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="29"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1023,8 +1015,8 @@
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="13"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="29"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1037,8 +1029,8 @@
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="13"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="29"/>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1051,8 +1043,8 @@
       <c r="E22" s="6"/>
       <c r="F22" s="7"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="13"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="29"/>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1065,8 +1057,8 @@
       <c r="E23" s="6"/>
       <c r="F23" s="7"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="13"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="29"/>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1079,8 +1071,8 @@
       <c r="E24" s="6"/>
       <c r="F24" s="7"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="13"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="29"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1093,8 +1085,8 @@
       <c r="E25" s="6"/>
       <c r="F25" s="7"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="13"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="29"/>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1107,9 +1099,10 @@
       <c r="E26" s="6"/>
       <c r="F26" s="7"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="13"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="29"/>
       <c r="J26" s="2"/>
+      <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
@@ -1121,8 +1114,8 @@
       <c r="E27" s="6"/>
       <c r="F27" s="7"/>
       <c r="G27" s="6"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="13"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="29"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1135,8 +1128,8 @@
       <c r="E28" s="6"/>
       <c r="F28" s="7"/>
       <c r="G28" s="6"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="13"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="29"/>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1149,8 +1142,8 @@
       <c r="E29" s="6"/>
       <c r="F29" s="7"/>
       <c r="G29" s="6"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="13"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="29"/>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1163,8 +1156,8 @@
       <c r="E30" s="6"/>
       <c r="F30" s="7"/>
       <c r="G30" s="6"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="13"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="29"/>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1177,8 +1170,8 @@
       <c r="E31" s="6"/>
       <c r="F31" s="7"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="13"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="29"/>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1191,8 +1184,8 @@
       <c r="E32" s="6"/>
       <c r="F32" s="7"/>
       <c r="G32" s="6"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="13"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="29"/>
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,130 +1198,147 @@
       <c r="E33" s="6"/>
       <c r="F33" s="7"/>
       <c r="G33" s="6"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="13"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E37" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="22" t="s">
+      <c r="H37" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="23"/>
+      <c r="I37" s="24"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="26"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="26"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="25"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="18"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="26"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="19">
+        <f>SUM(B3:B33)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="19">
+        <f>SUM(D3:D33)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="19">
+        <f>SUM(C39:D39)</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="20">
+        <f>SUM(H3:H33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="H39" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="I39" s="18"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="26"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="19"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="H41" s="20" t="s">
+      <c r="C41" s="19">
+        <f>SUM(C3:C33)</f>
+        <v>0</v>
+      </c>
+      <c r="D41" s="19">
+        <f>SUM(E3:E33)</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="19">
+        <f>SUM(C41:D41)</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I41" s="18" t="s">
-        <v>16</v>
+      <c r="I41" s="20">
+        <f>SUM(I3:I33)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="26"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
       <c r="H42" s="21"/>
-      <c r="I42" s="19"/>
+      <c r="I42" s="21"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="17" t="s">
-        <v>27</v>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="17" t="s">
-        <v>27</v>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-      <c r="I49" s="17" t="s">
-        <v>27</v>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H37:I38"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="D39:D40"/>
@@ -1336,11 +1346,16 @@
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="E41:E42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H37:I38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1365,38 +1380,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="11" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
melhorando o ux da planilha
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -145,15 +145,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -358,81 +349,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -718,571 +725,560 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39:I40"/>
+      <selection activeCell="C41" sqref="C41:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="29" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="29" t="s">
+      <c r="E3" s="18"/>
+      <c r="F3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="29" t="s">
+      <c r="G3" s="18"/>
+      <c r="H3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="30"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="5" t="s">
+      <c r="I3" s="18"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="19"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="29"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="19"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="B7" s="5"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="B8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="19"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="B10" s="5"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="19"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="19"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="19"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="B13" s="5"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="19"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="B14" s="5"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="19"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="19"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
         <v>13</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="19"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="B17" s="5"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="19"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="B18" s="5"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="2"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="B19" s="5"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
         <v>16</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="B20" s="5"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="B21" s="5"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <v>18</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>19</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="B23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>20</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="B24" s="5"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="16"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
         <v>21</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="16"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
         <v>22</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
         <v>23</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
         <v>24</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="B28" s="5"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
         <v>25</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
+      <c r="B29" s="5"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="16"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <v>26</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="B30" s="5"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
         <v>27</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="B31" s="5"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="16"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
         <v>28</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="B32" s="5"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="16"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
         <v>29</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="B33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="16"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
         <v>30</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="B34" s="5"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="16"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
         <v>31</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="19"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="16"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="H37" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="24"/>
+      <c r="I37" s="26"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="27"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="27"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="26"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="20"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="28"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="28">
-        <f>SUM(B3:B33)</f>
+      <c r="C39" s="21">
+        <f>SUM(B5:B35)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="28">
-        <f>SUM(D3:D33)</f>
+      <c r="D39" s="21">
+        <f>SUM(D5:D35)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="28">
+      <c r="E39" s="21">
         <f>SUM(C39:D39)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="22" t="s">
+      <c r="H39" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="I39" s="20">
-        <f>SUM(H3:H33)</f>
+      <c r="I39" s="22">
+        <f>SUM(H5:H35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="28"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="28">
-        <f>SUM(C3:C33)</f>
+      <c r="C41" s="21">
+        <f>SUM(C5:C35)</f>
         <v>0</v>
       </c>
-      <c r="D41" s="28">
-        <f>SUM(E3:E33)</f>
+      <c r="D41" s="21">
+        <f>SUM(E5:E35)</f>
         <v>0</v>
       </c>
-      <c r="E41" s="28">
+      <c r="E41" s="21">
         <f>SUM(C41:D41)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="22" t="s">
+      <c r="H41" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I41" s="20">
-        <f>SUM(I3:I33)</f>
+      <c r="I41" s="22">
+        <f>SUM(I5:I35)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="27"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
@@ -1290,53 +1286,49 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="14" t="s">
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="14" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="14" t="s">
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="12" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="B39:B40"/>
+  <mergeCells count="23">
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="H37:I38"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="D39:D40"/>
@@ -1344,11 +1336,16 @@
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="E41:E42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H37:I38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1374,40 +1371,40 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="9" width="9.140625" style="16"/>
+    <col min="8" max="9" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>